<commit_message>
enhance testing import format, more fields, more informations
</commit_message>
<xml_diff>
--- a/bookbag/testing/data/courseware.xlsx
+++ b/bookbag/testing/data/courseware.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33220" yWindow="600" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="课件" sheetId="2" r:id="rId1"/>
     <sheet name="工作表1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,73 +20,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>1.ppt</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>一班</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>答题卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人教</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新学案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit 1-Period 1.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>teacher1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一班</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教师</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>班级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>年级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>版本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>课件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>答题卡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test.xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人教</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>课程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语文</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -131,9 +135,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
@@ -468,75 +478,78 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -551,7 +564,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>